<commit_message>
final draft for submission
</commit_message>
<xml_diff>
--- a/manuscript/Literature_review.xlsx
+++ b/manuscript/Literature_review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbsbr11/Documents/1.research/1.research_papers/2.active/Forecasting_EPSS_domain_knowledge/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D364CEDF-36BD-2F4B-8E01-E4DA6FE22987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8474BD7-204A-FB43-B1A7-3AA1AA74C24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22700" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>Metric</t>
   </si>
   <si>
-    <t>ARIMA, HOLT’S WINTER, ETS,  Theta, ARHOW</t>
-  </si>
-  <si>
     <t>MEAN, MAD, MSE, RMSE,  MAPE</t>
   </si>
   <si>
@@ -115,21 +112,12 @@
     <t>MA, Symbolic Regression, LR</t>
   </si>
   <si>
-    <t>Diffusion models,  ARIMA,ES, LR</t>
-  </si>
-  <si>
     <t>ARIMA, ETS, MLP, SVR, RF, LR</t>
   </si>
   <si>
-    <t>MA, LR,Clustering and RNN</t>
-  </si>
-  <si>
     <t>6 Month MA, SES, WES</t>
   </si>
   <si>
-    <t xml:space="preserve">SES, MA, Naïve, Holt‘s linear </t>
-  </si>
-  <si>
     <t>NF</t>
   </si>
   <si>
@@ -142,9 +130,6 @@
     <t>HW-M</t>
   </si>
   <si>
-    <t>Naïve, Seasonal Naïve,ARIMA, DLM, LST, Recurrent Neural Network, SES, Holts  linear and damped trends, HW, ES-SSM, Theta</t>
-  </si>
-  <si>
     <t>ARIMA, ES</t>
   </si>
   <si>
@@ -355,18 +340,12 @@
     <t>1095 days</t>
   </si>
   <si>
-    <t>three exponential smoothing methods (Brown’s method, Holt’s method, and Holt-Winters method) along with a moving average model.</t>
-  </si>
-  <si>
     <t>MAD, MAPE</t>
   </si>
   <si>
     <t>1 year</t>
   </si>
   <si>
-    <t>Naïve,ARIMA,XGBoost ,LSTM neural networks, Prophet model</t>
-  </si>
-  <si>
     <t>Konstantinos  et al.(2024)</t>
   </si>
   <si>
@@ -403,9 +382,6 @@
     <t>Consumption</t>
   </si>
   <si>
-    <t>TimeGpt (with and without predictors), LSTM (with and without predictors), Exponntial Smoothing, ARIMA, Dynamic Regrssion (ARIMAX), Multiple Regression (with and without predictors)</t>
-  </si>
-  <si>
     <t>Sales of pharmaceutical products</t>
   </si>
   <si>
@@ -419,6 +395,30 @@
   </si>
   <si>
     <t>drug distribution</t>
+  </si>
+  <si>
+    <t>TimeGpt (with and without predictors), LSTM (with and without predictors), Exponential Smoothing, ARIMA, Dynamic Regression (ARIMAX), Multiple Regression (with and without predictors)</t>
+  </si>
+  <si>
+    <t>ARIMA, HOLT WINTER, ETS,  Theta, ARHOW</t>
+  </si>
+  <si>
+    <t>Diffusion models,  ARIMA, ES, LR</t>
+  </si>
+  <si>
+    <t>MA, LR, Clustering and RNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SES, MA, Naïve, Holt  </t>
+  </si>
+  <si>
+    <t>Naïve, Seasonal Naïve, ARIMA, DLM, LST, Recurrent Neural Network, SES, Holts linear and damped trends, HW, ES-SSM, Theta</t>
+  </si>
+  <si>
+    <t>Brown’s method, Holt’s method, and Holt-Winters method, moving average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naïve, ARIMA, XGBoost , LSTM, Prophet </t>
   </si>
 </sst>
 </file>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,19 +880,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -901,783 +901,783 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>90</v>
-      </c>
       <c r="G2" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I2" s="13">
         <v>33</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="I3" s="4">
         <v>31</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" s="8">
         <v>11</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="I5" s="6">
         <v>57</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="I6" s="6">
         <v>4</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I7" s="6">
         <v>1</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I8" s="6">
         <v>14</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="6">
         <v>50</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="6">
         <v>217</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" s="6">
         <v>245</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12" s="6">
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I13" s="6">
         <v>8</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="I14" s="6">
         <v>1</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="I15" s="6">
         <v>357</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I16" s="6">
         <v>1</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" s="6">
         <v>1</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I18" s="6">
         <v>30</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="I19" s="6">
         <v>1</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B22" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>110</v>
-      </c>
       <c r="D22" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I22" s="15">
         <v>125</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="I23" s="15">
         <v>57</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>